<commit_message>
added sky output temperature data processing and cleansing
</commit_message>
<xml_diff>
--- a/input/RESULTS5-2A-CSE-0.861.1.xlsx
+++ b/input/RESULTS5-2A-CSE-0.861.1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="171">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -2233,11 +2233,11 @@
   </sheetPr>
   <dimension ref="A3:AO579"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A302" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C330" activeCellId="0" sqref="C330"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A153" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A169" activeCellId="0" sqref="A169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>
@@ -4990,19 +4990,37 @@
         <v>40</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="C178" s="105"/>
-      <c r="D178" s="106"/>
-      <c r="E178" s="68"/>
-      <c r="F178" s="106"/>
-      <c r="G178" s="106"/>
-      <c r="H178" s="107"/>
-      <c r="I178" s="68"/>
-      <c r="J178" s="106"/>
-      <c r="K178" s="108"/>
+      <c r="C178" s="105" t="n">
+        <v>-3.93067013428873</v>
+      </c>
+      <c r="D178" s="106" t="n">
+        <v>-46.22457</v>
+      </c>
+      <c r="E178" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="F178" s="106" t="n">
+        <v>31</v>
+      </c>
+      <c r="G178" s="106" t="n">
+        <v>24</v>
+      </c>
+      <c r="H178" s="107" t="n">
+        <v>30.08121</v>
+      </c>
+      <c r="I178" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="J178" s="106" t="n">
+        <v>13</v>
+      </c>
+      <c r="K178" s="108" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E179" s="13" t="s">

</xml_diff>